<commit_message>
categorisation of risks added
</commit_message>
<xml_diff>
--- a/3_Backcasting analysis/analysis/Selection of risks and associated likelihood.xlsx
+++ b/3_Backcasting analysis/analysis/Selection of risks and associated likelihood.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kvase0-my.sharepoint.com/personal/loudel30_kva_se/Documents/Dokument/GitHub/WEF-GRR-analysis/3_Backcasting analysis/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2804" documentId="13_ncr:1_{6CDB6784-CF0F-4546-AE62-A0BDC9273E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDE96666-72D0-4757-9010-5DF02630D10C}"/>
+  <xr:revisionPtr revIDLastSave="2806" documentId="13_ncr:1_{6CDB6784-CF0F-4546-AE62-A0BDC9273E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79D51ABC-9A35-4235-BAFE-4B40B0AF8B09}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="799" xr2:uid="{959A7320-51B1-1040-BF09-D955BFA7AAAD}"/>
   </bookViews>
@@ -2620,8 +2620,8 @@
   </sheetPr>
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="89" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2984,7 +2984,7 @@
       </c>
       <c r="G10" s="2">
         <f>'2014'!H46</f>
-        <v>3.3785594639865968</v>
+        <v>3.1809045226130621</v>
       </c>
       <c r="H10" s="2">
         <f>'2014'!I46</f>
@@ -3955,7 +3955,7 @@
       </c>
       <c r="G44" s="3">
         <f>CORREL(G2:G17,G21:G36)</f>
-        <v>-0.43246506487897191</v>
+        <v>-0.4427784293962993</v>
       </c>
       <c r="H44" s="3">
         <f>CORREL(H2:H17,H21:H36)</f>
@@ -3995,7 +3995,7 @@
       </c>
       <c r="G45" s="3">
         <f>CORREL(G2:G17,G22:G37)</f>
-        <v>-0.36431998282941108</v>
+        <v>-0.35240066954757249</v>
       </c>
       <c r="H45" s="3">
         <f>CORREL(H2:H17,H22:H37)</f>
@@ -4035,7 +4035,7 @@
       </c>
       <c r="G46" s="3">
         <f>CORREL(G2:G17,G23:G38)</f>
-        <v>-0.41551215356801496</v>
+        <v>-0.41182579399509167</v>
       </c>
       <c r="H46" s="3">
         <f>CORREL(H2:H17,H23:H38)</f>
@@ -4075,7 +4075,7 @@
       </c>
       <c r="G47" s="3">
         <f>CORREL(G2:G17,G24:G39)</f>
-        <v>8.5038548459529462E-2</v>
+        <v>8.730694476936568E-2</v>
       </c>
       <c r="H47" s="3">
         <f>CORREL(H2:H17,H24:H39)</f>
@@ -4115,7 +4115,7 @@
       </c>
       <c r="G48" s="3">
         <f>CORREL(G2:G17,G25:G40)</f>
-        <v>0.26106008261566516</v>
+        <v>0.27829952442367312</v>
       </c>
       <c r="H48" s="3">
         <f>CORREL(H2:H17,H25:H40)</f>
@@ -4155,7 +4155,7 @@
       </c>
       <c r="G49" s="3">
         <f>CORREL(G2:G16,G27:G41)</f>
-        <v>-0.23130219396004947</v>
+        <v>-0.24341476801093154</v>
       </c>
       <c r="H49" s="3">
         <f>CORREL(H2:H16,H27:H41)</f>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="G50" s="3">
         <f>CORREL(G2:G15,G28:G41)</f>
-        <v>-0.49846368026054566</v>
+        <v>-0.49667160788701709</v>
       </c>
       <c r="H50" s="3">
         <f>CORREL(H2:H15,H28:H41)</f>
@@ -4235,7 +4235,7 @@
       </c>
       <c r="G51" s="3">
         <f>CORREL(G2:G14,G29:G41)</f>
-        <v>-0.46349999785856627</v>
+        <v>-0.44839814119934723</v>
       </c>
       <c r="H51" s="3">
         <f>CORREL(H2:H14,H29:H41)</f>
@@ -4275,7 +4275,7 @@
       </c>
       <c r="G52" s="3">
         <f>CORREL(G2:G13,G30:G41)</f>
-        <v>-0.47312892292265246</v>
+        <v>-0.46188791029751769</v>
       </c>
       <c r="H52" s="3">
         <f>CORREL(H2:H13,H30:H41)</f>
@@ -4315,7 +4315,7 @@
       </c>
       <c r="G53" s="3">
         <f>CORREL(G2:G12,G31:G41)</f>
-        <v>-8.930838856860053E-2</v>
+        <v>-1.5138876030639263E-2</v>
       </c>
       <c r="H53" s="3">
         <f>CORREL(H2:H12,H31:H41)</f>
@@ -4352,7 +4352,7 @@
       </c>
       <c r="G56" s="4">
         <f t="shared" si="3"/>
-        <v>-0.17323971404024066</v>
+        <v>-0.16827968474918495</v>
       </c>
       <c r="H56" s="4">
         <f t="shared" si="3"/>
@@ -4368,7 +4368,7 @@
       </c>
       <c r="K56" s="4">
         <f>AVERAGE(C56:J56)</f>
-        <v>-0.1284343948718501</v>
+        <v>-0.12781439121046814</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -4393,7 +4393,7 @@
       </c>
       <c r="G57" s="4">
         <f t="shared" si="4"/>
-        <v>-0.35114063671408291</v>
+        <v>-0.33310226068509052</v>
       </c>
       <c r="H57" s="4">
         <f t="shared" si="4"/>
@@ -4409,7 +4409,7 @@
       </c>
       <c r="K57" s="4">
         <f>AVERAGE(C57:J57)</f>
-        <v>4.062606020043269E-4</v>
+        <v>2.6610576056283752E-3</v>
       </c>
     </row>
   </sheetData>
@@ -4436,8 +4436,8 @@
   </sheetPr>
   <dimension ref="A1:L533"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView topLeftCell="A294" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I315" sqref="I315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -11356,9 +11356,7 @@
       <c r="F315" s="2"/>
       <c r="G315" s="2"/>
       <c r="H315" s="2"/>
-      <c r="I315" s="2">
-        <v>1</v>
-      </c>
+      <c r="I315" s="2"/>
       <c r="J315" s="2"/>
       <c r="K315" s="2"/>
       <c r="L315" s="2"/>
@@ -22708,8 +22706,8 @@
   </sheetPr>
   <dimension ref="A2:T46"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:K42"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -23349,9 +23347,6 @@
       <c r="C34" s="10">
         <v>3.9715242881072004</v>
       </c>
-      <c r="H34" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="35" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A35" s="39" t="s">
@@ -23410,7 +23405,7 @@
       </c>
       <c r="H38" s="2">
         <f t="shared" si="3"/>
-        <v>3.9715242881072004</v>
+        <v>0</v>
       </c>
       <c r="I38" s="2">
         <f t="shared" si="3"/>
@@ -23560,7 +23555,7 @@
       </c>
       <c r="H45" s="2">
         <f t="shared" si="5"/>
-        <v>13.514237855946387</v>
+        <v>9.5427135678391863</v>
       </c>
       <c r="I45" s="2">
         <f t="shared" si="5"/>
@@ -23594,7 +23589,7 @@
       </c>
       <c r="H46" s="2">
         <f t="shared" si="6"/>
-        <v>3.3785594639865968</v>
+        <v>3.1809045226130621</v>
       </c>
       <c r="I46" s="2">
         <f t="shared" si="6"/>
@@ -37488,8 +37483,8 @@
   </sheetPr>
   <dimension ref="A2:T52"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:K49"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>